<commit_message>
Allow mapping strings and support equality comparers
</commit_message>
<xml_diff>
--- a/src/ExcelMapper.Tests/Resources/Primitives.xlsx
+++ b/src/ExcelMapper.Tests/Resources/Primitives.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>Int Value</t>
   </si>
@@ -80,6 +80,15 @@
   </si>
   <si>
     <t>a;b;c,d;e</t>
+  </si>
+  <si>
+    <t>MappedValue</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>D</t>
   </si>
 </sst>
 </file>
@@ -399,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="G1:K5"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -414,7 +423,7 @@
     <col min="7" max="9" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -433,8 +442,11 @@
       <c r="F1" t="s">
         <v>15</v>
       </c>
+      <c r="G1" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -453,8 +465,11 @@
       <c r="F2" t="s">
         <v>16</v>
       </c>
+      <c r="G2" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -470,8 +485,11 @@
       <c r="E3" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="G3" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -481,8 +499,11 @@
       <c r="F4" t="s">
         <v>3</v>
       </c>
+      <c r="G4" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>5</v>
       </c>
@@ -497,6 +518,9 @@
       </c>
       <c r="F5" t="s">
         <v>17</v>
+      </c>
+      <c r="G5" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>